<commit_message>
Complete below automation work for EmployeeTest.java
</commit_message>
<xml_diff>
--- a/test-data/orange-data.xlsx
+++ b/test-data/orange-data.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="1"/>
+    <workbookView xWindow="204" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="invalidLoginTest" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="addValidEmployeeTest" sheetId="3" r:id="rId3"/>
     <sheet name="validLoginTest" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Username</t>
   </si>
@@ -53,13 +53,34 @@
   </si>
   <si>
     <t>Quick Launch</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>Wick</t>
+  </si>
+  <si>
+    <t>Jack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -70,6 +91,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -93,9 +121,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,7 +352,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -375,13 +404,68 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>